<commit_message>
add import_traffic function to import Excel file with all road data and settings
</commit_message>
<xml_diff>
--- a/tests/edb/data/TrafficImportFormat.xlsx
+++ b/tests/edb/data/TrafficImportFormat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,7 @@
     <sheet name="TrafficSituation" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="VehicleEmissionFactor" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="CodeSet" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="ActivityCode" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="173">
   <si>
     <t xml:space="preserve">Each road (segment) has an assigned fleet and traffic situation, where the traffic situation itself can be defined by multiple attributes.</t>
   </si>
@@ -444,6 +445,9 @@
     <t xml:space="preserve">fleet</t>
   </si>
   <si>
+    <t xml:space="preserve">speed</t>
+  </si>
+  <si>
     <t xml:space="preserve">congestion_profile</t>
   </si>
   <si>
@@ -477,12 +481,12 @@
     <t xml:space="preserve">andel_lb</t>
   </si>
   <si>
-    <t xml:space="preserve">IPA_Funkkl</t>
-  </si>
-  <si>
     <t xml:space="preserve">IPA_Hastig</t>
   </si>
   <si>
+    <t xml:space="preserve">roadtype</t>
+  </si>
+  <si>
     <t xml:space="preserve">KOMMUNKOD</t>
   </si>
   <si>
@@ -513,7 +517,7 @@
     <t xml:space="preserve">petrol</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3.1</t>
+    <t xml:space="preserve">1.A.3.b</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -531,9 +535,6 @@
     <t xml:space="preserve">A lorry</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">motorcycle</t>
   </si>
   <si>
@@ -717,24 +718,12 @@
     <t xml:space="preserve">December</t>
   </si>
   <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
     <t xml:space="preserve">slug</t>
   </si>
   <si>
-    <t xml:space="preserve">roadtype</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> roadtype</t>
-  </si>
-  <si>
     <t xml:space="preserve">posted speed</t>
   </si>
   <si>
-    <t xml:space="preserve"> speed</t>
-  </si>
-  <si>
     <t xml:space="preserve">traffic_situation</t>
   </si>
   <si>
@@ -787,6 +776,63 @@
   </si>
   <si>
     <t xml:space="preserve">NFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codeset_slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activitycode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, passenger cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.ii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, light duty vehicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.iii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, heavy duty vehicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.iv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, mopeds &amp; motorcycles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, gasoline evaporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, automobile tyre and brake wear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.3.b.vii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport, automobile road abrasion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transport</t>
   </si>
 </sst>
 </file>
@@ -937,7 +983,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1107,7 +1153,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1117,7 +1163,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1158,23 +1204,23 @@
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>21</v>
@@ -1189,24 +1235,24 @@
         <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>100</v>
@@ -1224,24 +1270,24 @@
         <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>100</v>
@@ -1262,16 +1308,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>100</v>
@@ -1292,16 +1338,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>100</v>
@@ -1322,16 +1368,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>100</v>
@@ -1352,16 +1398,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>100</v>
@@ -1441,41 +1487,175 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1494,18 +1674,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,37 +1726,43 @@
       <c r="L1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>55</v>
+      </c>
       <c r="K2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>56</v>
+      <c r="M2" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1597,10 +1784,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.36"/>
   </cols>
@@ -1610,79 +1797,79 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,19 +1877,19 @@
         <v>73</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +1914,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
@@ -1777,7 +1964,7 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0.9</v>
@@ -1832,7 +2019,7 @@
         <v>0.1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -1858,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -1901,7 +2088,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3237,7 +3424,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3993,10 +4180,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4029,7 +4216,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>96</v>
@@ -4697,40 +4884,40 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="3" t="n">
-        <v>21.7920946997267</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>11.0721371882086</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>4.44159787371827</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="n">
-        <v>2.2491308233933</v>
+        <v>1</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>1.27666930256322</v>
+        <v>1</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>0.890170734746924</v>
+        <v>1</v>
       </c>
       <c r="I27" s="3" t="n">
-        <v>0.73624300495521</v>
+        <v>1</v>
       </c>
       <c r="J27" s="3" t="n">
-        <v>0.720673351056132</v>
+        <v>1</v>
       </c>
       <c r="K27" s="3" t="n">
-        <v>1.04729039791799</v>
+        <v>1</v>
       </c>
       <c r="L27" s="3" t="n">
-        <v>1.7906763778628</v>
+        <v>1</v>
       </c>
       <c r="M27" s="3" t="n">
-        <v>3.95764997910361</v>
+        <v>1</v>
       </c>
       <c r="N27" s="3" t="n">
-        <v>12.9654263939778</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4752,10 +4939,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.16"/>
   </cols>
@@ -4765,23 +4952,23 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -4800,34 +4987,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -4835,10 +5022,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>70</v>
@@ -4846,10 +5033,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>90</v>
@@ -4857,10 +5044,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>50</v>
@@ -4868,10 +5055,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>70</v>
@@ -4879,13 +5066,145 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix error in TrafficImportFormat for tests
</commit_message>
<xml_diff>
--- a/tests/edb/data/TrafficImportFormat.xlsx
+++ b/tests/edb/data/TrafficImportFormat.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="171">
   <si>
     <t xml:space="preserve">Each road (segment) has an assigned fleet and traffic situation, where the traffic situation itself can be defined by multiple attributes.</t>
   </si>
@@ -481,12 +481,12 @@
     <t xml:space="preserve">andel_lb</t>
   </si>
   <si>
+    <t xml:space="preserve">roadtype</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPA_Hastig</t>
   </si>
   <si>
-    <t xml:space="preserve">roadtype</t>
-  </si>
-  <si>
     <t xml:space="preserve">KOMMUNKOD</t>
   </si>
   <si>
@@ -565,13 +565,13 @@
     <t xml:space="preserve">fuel:diesel</t>
   </si>
   <si>
-    <t xml:space="preserve">Motorway urban</t>
+    <t xml:space="preserve">motorway</t>
   </si>
   <si>
     <t xml:space="preserve">constant</t>
   </si>
   <si>
-    <t xml:space="preserve">Motorway rural</t>
+    <t xml:space="preserve">primary road</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -733,15 +733,9 @@
     <t xml:space="preserve">1a</t>
   </si>
   <si>
-    <t xml:space="preserve">motorway</t>
-  </si>
-  <si>
     <t xml:space="preserve">1b</t>
   </si>
   <si>
-    <t xml:space="preserve">primary road</t>
-  </si>
-  <si>
     <t xml:space="preserve">substance</t>
   </si>
   <si>
@@ -755,9 +749,6 @@
   </si>
   <si>
     <t xml:space="preserve">mg/km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">import function expects same unit for all! Can force to only have unit on first row?</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
@@ -986,7 +977,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1204,10 +1195,10 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.69"/>
   </cols>
@@ -1223,7 +1214,7 @@
         <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>21</v>
@@ -1238,10 +1229,10 @@
         <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,7 +1246,7 @@
         <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>100</v>
@@ -1273,15 +1264,13 @@
         <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>63</v>
@@ -1290,7 +1279,7 @@
         <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>100</v>
@@ -1307,7 +1296,9 @@
       <c r="I3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1320,7 +1311,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>100</v>
@@ -1337,11 +1328,13 @@
       <c r="I4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>63</v>
@@ -1350,7 +1343,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>100</v>
@@ -1367,7 +1360,9 @@
       <c r="I5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1380,7 +1375,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>100</v>
@@ -1397,11 +1392,13 @@
       <c r="I6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>70</v>
@@ -1410,7 +1407,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>100</v>
@@ -1427,7 +1424,9 @@
       <c r="I7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="4"/>
@@ -1490,7 +1489,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1500,31 +1499,31 @@
         <v>134</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1549,116 +1548,116 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1679,11 +1678,11 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.06"/>
@@ -1755,14 +1754,17 @@
       <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>55</v>
+      </c>
       <c r="I2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>57</v>
@@ -1790,7 +1792,7 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.36"/>
   </cols>
@@ -1914,10 +1916,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
@@ -2091,7 +2093,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3427,7 +3429,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4186,7 +4188,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4945,7 +4947,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.16"/>
   </cols>
@@ -4963,7 +4965,7 @@
         <v>135</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4996,7 +4998,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.47"/>
   </cols>
@@ -5017,7 +5019,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -5028,7 +5030,7 @@
         <v>138</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>70</v>
@@ -5039,7 +5041,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>90</v>
@@ -5047,10 +5049,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>50</v>
@@ -5058,10 +5060,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>70</v>
@@ -5069,10 +5071,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>90</v>
@@ -5080,10 +5082,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>60</v>
@@ -5091,10 +5093,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>80</v>
@@ -5102,10 +5104,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>30</v>
@@ -5116,7 +5118,7 @@
         <v>138</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>100</v>
@@ -5127,7 +5129,7 @@
         <v>138</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>110</v>
@@ -5135,10 +5137,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>20</v>
@@ -5146,10 +5148,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>40</v>
@@ -5157,10 +5159,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>110</v>
@@ -5168,10 +5170,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>100</v>
@@ -5179,10 +5181,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -5190,10 +5192,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>5</v>
@@ -5201,10 +5203,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>120</v>

</xml_diff>